<commit_message>
fix macro_js and macro_jmp commands
</commit_message>
<xml_diff>
--- a/doc/controls.xlsx
+++ b/doc/controls.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="20480" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="20480" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="COMMANDS" sheetId="3" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="235">
   <si>
     <t>#</t>
   </si>
@@ -720,6 +720,21 @@
   </si>
   <si>
     <t>00010110</t>
+  </si>
+  <si>
+    <t>00101000</t>
+  </si>
+  <si>
+    <t>00101100</t>
+  </si>
+  <si>
+    <t>00001000</t>
+  </si>
+  <si>
+    <t>00000100</t>
+  </si>
+  <si>
+    <t>FLAG_RESET</t>
   </si>
 </sst>
 </file>
@@ -814,7 +829,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="725">
+  <cellStyleXfs count="733">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1540,8 +1555,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1603,6 +1626,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1615,14 +1647,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="725">
+  <cellStyles count="733">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1985,6 +2017,10 @@
     <cellStyle name="Followed Hyperlink" xfId="720" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="722" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="724" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="726" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="728" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="730" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="732" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2347,6 +2383,10 @@
     <cellStyle name="Hyperlink" xfId="719" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="721" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="723" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="725" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="727" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="729" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="731" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2649,7 +2689,7 @@
   <dimension ref="A1:P31"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2682,22 +2722,22 @@
         <v>75</v>
       </c>
       <c r="F1" s="20"/>
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29" t="s">
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="31" t="s">
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
+      <c r="O1" s="34"/>
+      <c r="P1" s="34"/>
     </row>
     <row r="2" spans="1:16">
       <c r="A2" s="11">
@@ -2714,24 +2754,24 @@
         <v>000001</v>
       </c>
       <c r="F2" s="10"/>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="J2" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" s="11">
@@ -2754,13 +2794,13 @@
       <c r="G3" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="I3" s="14">
+      <c r="I3" s="37">
         <v>5</v>
       </c>
-      <c r="J3" s="14">
+      <c r="J3" s="37">
         <v>6</v>
       </c>
       <c r="K3" s="21" t="s">
@@ -2808,13 +2848,13 @@
       <c r="G4" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="I4" s="11">
+      <c r="I4" s="15">
         <v>5</v>
       </c>
-      <c r="J4" s="11">
+      <c r="J4" s="15">
         <v>6</v>
       </c>
       <c r="K4" s="17" t="s">
@@ -2833,7 +2873,7 @@
         <v>0011</v>
       </c>
       <c r="O4" s="11" t="str">
-        <f t="shared" ref="O4:O18" si="5">BIN2HEX(L4,4)</f>
+        <f t="shared" ref="O4:O15" si="5">BIN2HEX(L4,4)</f>
         <v>0005</v>
       </c>
       <c r="P4" s="11" t="str">
@@ -2863,13 +2903,13 @@
       <c r="G5" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="29" t="s">
         <v>228</v>
       </c>
-      <c r="I5" s="11">
+      <c r="I5" s="15">
         <v>12</v>
       </c>
-      <c r="J5" s="11">
+      <c r="J5" s="15">
         <v>0</v>
       </c>
       <c r="K5" s="17" t="s">
@@ -2918,13 +2958,13 @@
       <c r="G6" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="I6" s="11">
+      <c r="I6" s="15">
         <v>6</v>
       </c>
-      <c r="J6" s="11">
+      <c r="J6" s="15">
         <v>0</v>
       </c>
       <c r="K6" s="17" t="s">
@@ -2973,13 +3013,13 @@
       <c r="G7" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="H7" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="I7" s="11">
+      <c r="I7" s="15">
         <v>19</v>
       </c>
-      <c r="J7" s="11">
+      <c r="J7" s="15">
         <v>0</v>
       </c>
       <c r="K7" s="17" t="s">
@@ -3028,13 +3068,13 @@
       <c r="G8" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H8" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="I8" s="11">
+      <c r="I8" s="15">
         <v>32</v>
       </c>
-      <c r="J8" s="11">
+      <c r="J8" s="15">
         <v>0</v>
       </c>
       <c r="K8" s="17" t="s">
@@ -3083,13 +3123,13 @@
       <c r="G9" s="11" t="s">
         <v>179</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="H9" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="I9" s="11">
+      <c r="I9" s="15">
         <v>32</v>
       </c>
-      <c r="J9" s="11">
+      <c r="J9" s="15">
         <v>0</v>
       </c>
       <c r="K9" s="17" t="s">
@@ -3136,39 +3176,39 @@
         <v>8</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="H10" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="H10" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="I10" s="11">
-        <v>32</v>
-      </c>
-      <c r="J10" s="11">
-        <v>33</v>
+      <c r="I10" s="15">
+        <v>16</v>
+      </c>
+      <c r="J10" s="15">
+        <v>17</v>
       </c>
       <c r="K10" s="17" t="s">
-        <v>215</v>
+        <v>230</v>
       </c>
       <c r="L10" s="16" t="str">
         <f t="shared" si="2"/>
-        <v>00100000</v>
+        <v>00010000</v>
       </c>
       <c r="M10" s="16" t="str">
         <f t="shared" si="3"/>
-        <v>00100001</v>
+        <v>00010001</v>
       </c>
       <c r="N10" s="11" t="str">
-        <f t="shared" si="4"/>
-        <v>0024</v>
+        <f>BIN2HEX(K10,4)</f>
+        <v>0028</v>
       </c>
       <c r="O10" s="11" t="str">
         <f t="shared" si="5"/>
-        <v>0020</v>
+        <v>0010</v>
       </c>
       <c r="P10" s="11" t="str">
         <f t="shared" si="6"/>
-        <v>0021</v>
+        <v>0011</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -3191,39 +3231,39 @@
         <v>9</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>213</v>
-      </c>
-      <c r="H11" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="H11" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="I11" s="11">
-        <v>40</v>
-      </c>
-      <c r="J11" s="11">
-        <v>0</v>
+      <c r="I11" s="15">
+        <v>16</v>
+      </c>
+      <c r="J11" s="15">
+        <v>17</v>
       </c>
       <c r="K11" s="17" t="s">
-        <v>217</v>
+        <v>231</v>
       </c>
       <c r="L11" s="16" t="str">
         <f t="shared" si="2"/>
-        <v>00101000</v>
+        <v>00010000</v>
       </c>
       <c r="M11" s="16" t="str">
         <f t="shared" si="3"/>
-        <v>00000000</v>
+        <v>00010001</v>
       </c>
       <c r="N11" s="11" t="str">
-        <f t="shared" si="4"/>
-        <v>0018</v>
+        <f t="shared" ref="N11:N18" si="8">BIN2HEX(K11,4)</f>
+        <v>002C</v>
       </c>
       <c r="O11" s="11" t="str">
         <f t="shared" si="5"/>
-        <v>0028</v>
+        <v>0010</v>
       </c>
       <c r="P11" s="11" t="str">
         <f t="shared" si="6"/>
-        <v>0000</v>
+        <v>0011</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -3245,30 +3285,40 @@
         <f t="shared" si="7"/>
         <v>10</v>
       </c>
-      <c r="G12" s="11"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="17"/>
+      <c r="G12" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="H12" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="I12" s="15">
+        <v>32</v>
+      </c>
+      <c r="J12" s="15">
+        <v>33</v>
+      </c>
+      <c r="K12" s="17" t="s">
+        <v>215</v>
+      </c>
       <c r="L12" s="16" t="str">
         <f t="shared" si="2"/>
-        <v>00000000</v>
+        <v>00100000</v>
       </c>
       <c r="M12" s="16" t="str">
         <f t="shared" si="3"/>
-        <v>00000000</v>
+        <v>00100001</v>
       </c>
       <c r="N12" s="11" t="str">
-        <f t="shared" si="4"/>
-        <v>0000</v>
+        <f t="shared" si="8"/>
+        <v>0024</v>
       </c>
       <c r="O12" s="11" t="str">
         <f t="shared" si="5"/>
-        <v>0000</v>
+        <v>0020</v>
       </c>
       <c r="P12" s="11" t="str">
         <f t="shared" si="6"/>
-        <v>0000</v>
+        <v>0021</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -3290,11 +3340,21 @@
         <f t="shared" si="7"/>
         <v>11</v>
       </c>
-      <c r="G13" s="11"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="17"/>
+      <c r="G13" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="H13" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="I13" s="15">
+        <v>0</v>
+      </c>
+      <c r="J13" s="15">
+        <v>0</v>
+      </c>
+      <c r="K13" s="17" t="s">
+        <v>233</v>
+      </c>
       <c r="L13" s="16" t="str">
         <f t="shared" si="2"/>
         <v>00000000</v>
@@ -3304,8 +3364,8 @@
         <v>00000000</v>
       </c>
       <c r="N13" s="11" t="str">
-        <f t="shared" si="4"/>
-        <v>0000</v>
+        <f t="shared" si="8"/>
+        <v>0004</v>
       </c>
       <c r="O13" s="11" t="str">
         <f t="shared" si="5"/>
@@ -3335,26 +3395,36 @@
         <f t="shared" si="7"/>
         <v>12</v>
       </c>
-      <c r="G14" s="11"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="17"/>
+      <c r="G14" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="H14" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="I14" s="15">
+        <v>40</v>
+      </c>
+      <c r="J14" s="15">
+        <v>0</v>
+      </c>
+      <c r="K14" s="17" t="s">
+        <v>217</v>
+      </c>
       <c r="L14" s="16" t="str">
         <f t="shared" si="2"/>
-        <v>00000000</v>
+        <v>00101000</v>
       </c>
       <c r="M14" s="16" t="str">
         <f t="shared" si="3"/>
         <v>00000000</v>
       </c>
       <c r="N14" s="11" t="str">
-        <f t="shared" si="4"/>
-        <v>0000</v>
+        <f t="shared" si="8"/>
+        <v>0018</v>
       </c>
       <c r="O14" s="11" t="str">
         <f t="shared" si="5"/>
-        <v>0000</v>
+        <v>0028</v>
       </c>
       <c r="P14" s="11" t="str">
         <f t="shared" si="6"/>
@@ -3366,11 +3436,21 @@
         <f t="shared" si="7"/>
         <v>13</v>
       </c>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="17"/>
+      <c r="G15" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="H15" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="I15" s="15">
+        <v>0</v>
+      </c>
+      <c r="J15" s="15">
+        <v>0</v>
+      </c>
+      <c r="K15" s="17" t="s">
+        <v>232</v>
+      </c>
       <c r="L15" s="16" t="str">
         <f t="shared" si="2"/>
         <v>00000000</v>
@@ -3380,8 +3460,8 @@
         <v>00000000</v>
       </c>
       <c r="N15" s="11" t="str">
-        <f t="shared" si="4"/>
-        <v>0000</v>
+        <f t="shared" si="8"/>
+        <v>0008</v>
       </c>
       <c r="O15" s="11" t="str">
         <f t="shared" si="5"/>
@@ -3413,11 +3493,11 @@
         <v>00000000</v>
       </c>
       <c r="N16" s="11" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0000</v>
       </c>
       <c r="O16" s="11" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="O4:O18" si="9">BIN2HEX(L16,4)</f>
         <v>0000</v>
       </c>
       <c r="P16" s="11" t="str">
@@ -3444,11 +3524,11 @@
         <v>00000000</v>
       </c>
       <c r="N17" s="11" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0000</v>
       </c>
       <c r="O17" s="11" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0000</v>
       </c>
       <c r="P17" s="11" t="str">
@@ -3475,11 +3555,11 @@
         <v>00000000</v>
       </c>
       <c r="N18" s="11" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0000</v>
       </c>
       <c r="O18" s="11" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0000</v>
       </c>
       <c r="P18" s="11" t="str">
@@ -3688,72 +3768,72 @@
       <c r="D1" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="32"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="32"/>
-      <c r="X1" s="32"/>
-      <c r="Y1" s="32"/>
-      <c r="Z1" s="32"/>
-      <c r="AA1" s="32"/>
-      <c r="AB1" s="32"/>
-      <c r="AC1" s="32"/>
-      <c r="AD1" s="32"/>
-      <c r="AE1" s="32"/>
-      <c r="AF1" s="32"/>
-      <c r="AG1" s="32"/>
-      <c r="AH1" s="32"/>
-      <c r="AI1" s="32"/>
-      <c r="AJ1" s="32"/>
-      <c r="AK1" s="32"/>
-      <c r="AL1" s="32"/>
-      <c r="AM1" s="32"/>
-      <c r="AN1" s="32"/>
-      <c r="AO1" s="32"/>
-      <c r="AP1" s="32"/>
-      <c r="AQ1" s="32"/>
-      <c r="AR1" s="32"/>
-      <c r="AS1" s="32"/>
-      <c r="AT1" s="32"/>
-      <c r="AU1" s="32"/>
-      <c r="AV1" s="32"/>
-      <c r="AW1" s="32"/>
-      <c r="AX1" s="32"/>
-      <c r="AY1" s="32"/>
-      <c r="AZ1" s="32"/>
-      <c r="BA1" s="32"/>
-      <c r="BB1" s="32"/>
-      <c r="BC1" s="32"/>
-      <c r="BD1" s="32"/>
-      <c r="BE1" s="32"/>
-      <c r="BF1" s="32"/>
-      <c r="BG1" s="32"/>
-      <c r="BH1" s="32"/>
-      <c r="BI1" s="32"/>
-      <c r="BJ1" s="32"/>
-      <c r="BK1" s="32"/>
-      <c r="BL1" s="32"/>
-      <c r="BM1" s="32"/>
-      <c r="BN1" s="32"/>
-      <c r="BO1" s="32"/>
-      <c r="BP1" s="32"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
+      <c r="P1" s="35"/>
+      <c r="Q1" s="35"/>
+      <c r="R1" s="35"/>
+      <c r="S1" s="35"/>
+      <c r="T1" s="35"/>
+      <c r="U1" s="35"/>
+      <c r="V1" s="35"/>
+      <c r="W1" s="35"/>
+      <c r="X1" s="35"/>
+      <c r="Y1" s="35"/>
+      <c r="Z1" s="35"/>
+      <c r="AA1" s="35"/>
+      <c r="AB1" s="35"/>
+      <c r="AC1" s="35"/>
+      <c r="AD1" s="35"/>
+      <c r="AE1" s="35"/>
+      <c r="AF1" s="35"/>
+      <c r="AG1" s="35"/>
+      <c r="AH1" s="35"/>
+      <c r="AI1" s="35"/>
+      <c r="AJ1" s="35"/>
+      <c r="AK1" s="35"/>
+      <c r="AL1" s="35"/>
+      <c r="AM1" s="35"/>
+      <c r="AN1" s="35"/>
+      <c r="AO1" s="35"/>
+      <c r="AP1" s="35"/>
+      <c r="AQ1" s="35"/>
+      <c r="AR1" s="35"/>
+      <c r="AS1" s="35"/>
+      <c r="AT1" s="35"/>
+      <c r="AU1" s="35"/>
+      <c r="AV1" s="35"/>
+      <c r="AW1" s="35"/>
+      <c r="AX1" s="35"/>
+      <c r="AY1" s="35"/>
+      <c r="AZ1" s="35"/>
+      <c r="BA1" s="35"/>
+      <c r="BB1" s="35"/>
+      <c r="BC1" s="35"/>
+      <c r="BD1" s="35"/>
+      <c r="BE1" s="35"/>
+      <c r="BF1" s="35"/>
+      <c r="BG1" s="35"/>
+      <c r="BH1" s="35"/>
+      <c r="BI1" s="35"/>
+      <c r="BJ1" s="35"/>
+      <c r="BK1" s="35"/>
+      <c r="BL1" s="35"/>
+      <c r="BM1" s="35"/>
+      <c r="BN1" s="35"/>
+      <c r="BO1" s="35"/>
+      <c r="BP1" s="35"/>
     </row>
     <row r="2" spans="1:68">
       <c r="A2" s="10" t="s">
@@ -3868,10 +3948,10 @@
       </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="32"/>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
+      <c r="A28" s="35"/>
+      <c r="B28" s="35"/>
+      <c r="C28" s="35"/>
+      <c r="D28" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3879,7 +3959,6 @@
     <mergeCell ref="A28:D28"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3920,72 +3999,72 @@
       <c r="D1" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="32"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="32"/>
-      <c r="X1" s="32"/>
-      <c r="Y1" s="32"/>
-      <c r="Z1" s="32"/>
-      <c r="AA1" s="32"/>
-      <c r="AB1" s="32"/>
-      <c r="AC1" s="32"/>
-      <c r="AD1" s="32"/>
-      <c r="AE1" s="32"/>
-      <c r="AF1" s="32"/>
-      <c r="AG1" s="32"/>
-      <c r="AH1" s="32"/>
-      <c r="AI1" s="32"/>
-      <c r="AJ1" s="32"/>
-      <c r="AK1" s="32"/>
-      <c r="AL1" s="32"/>
-      <c r="AM1" s="32"/>
-      <c r="AN1" s="32"/>
-      <c r="AO1" s="32"/>
-      <c r="AP1" s="32"/>
-      <c r="AQ1" s="32"/>
-      <c r="AR1" s="32"/>
-      <c r="AS1" s="32"/>
-      <c r="AT1" s="32"/>
-      <c r="AU1" s="32"/>
-      <c r="AV1" s="32"/>
-      <c r="AW1" s="32"/>
-      <c r="AX1" s="32"/>
-      <c r="AY1" s="32"/>
-      <c r="AZ1" s="32"/>
-      <c r="BA1" s="32"/>
-      <c r="BB1" s="32"/>
-      <c r="BC1" s="32"/>
-      <c r="BD1" s="32"/>
-      <c r="BE1" s="32"/>
-      <c r="BF1" s="32"/>
-      <c r="BG1" s="32"/>
-      <c r="BH1" s="32"/>
-      <c r="BI1" s="32"/>
-      <c r="BJ1" s="32"/>
-      <c r="BK1" s="32"/>
-      <c r="BL1" s="32"/>
-      <c r="BM1" s="32"/>
-      <c r="BN1" s="32"/>
-      <c r="BO1" s="32"/>
-      <c r="BP1" s="32"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
+      <c r="P1" s="35"/>
+      <c r="Q1" s="35"/>
+      <c r="R1" s="35"/>
+      <c r="S1" s="35"/>
+      <c r="T1" s="35"/>
+      <c r="U1" s="35"/>
+      <c r="V1" s="35"/>
+      <c r="W1" s="35"/>
+      <c r="X1" s="35"/>
+      <c r="Y1" s="35"/>
+      <c r="Z1" s="35"/>
+      <c r="AA1" s="35"/>
+      <c r="AB1" s="35"/>
+      <c r="AC1" s="35"/>
+      <c r="AD1" s="35"/>
+      <c r="AE1" s="35"/>
+      <c r="AF1" s="35"/>
+      <c r="AG1" s="35"/>
+      <c r="AH1" s="35"/>
+      <c r="AI1" s="35"/>
+      <c r="AJ1" s="35"/>
+      <c r="AK1" s="35"/>
+      <c r="AL1" s="35"/>
+      <c r="AM1" s="35"/>
+      <c r="AN1" s="35"/>
+      <c r="AO1" s="35"/>
+      <c r="AP1" s="35"/>
+      <c r="AQ1" s="35"/>
+      <c r="AR1" s="35"/>
+      <c r="AS1" s="35"/>
+      <c r="AT1" s="35"/>
+      <c r="AU1" s="35"/>
+      <c r="AV1" s="35"/>
+      <c r="AW1" s="35"/>
+      <c r="AX1" s="35"/>
+      <c r="AY1" s="35"/>
+      <c r="AZ1" s="35"/>
+      <c r="BA1" s="35"/>
+      <c r="BB1" s="35"/>
+      <c r="BC1" s="35"/>
+      <c r="BD1" s="35"/>
+      <c r="BE1" s="35"/>
+      <c r="BF1" s="35"/>
+      <c r="BG1" s="35"/>
+      <c r="BH1" s="35"/>
+      <c r="BI1" s="35"/>
+      <c r="BJ1" s="35"/>
+      <c r="BK1" s="35"/>
+      <c r="BL1" s="35"/>
+      <c r="BM1" s="35"/>
+      <c r="BN1" s="35"/>
+      <c r="BO1" s="35"/>
+      <c r="BP1" s="35"/>
     </row>
     <row r="2" spans="1:68">
       <c r="A2" s="25" t="s">
@@ -4176,10 +4255,10 @@
       </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="32"/>
-      <c r="B27" s="32"/>
-      <c r="C27" s="32"/>
-      <c r="D27" s="32"/>
+      <c r="A27" s="35"/>
+      <c r="B27" s="35"/>
+      <c r="C27" s="35"/>
+      <c r="D27" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -4187,7 +4266,6 @@
     <mergeCell ref="A27:D27"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4228,72 +4306,72 @@
       <c r="E1" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="32"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="32"/>
-      <c r="X1" s="32"/>
-      <c r="Y1" s="32"/>
-      <c r="Z1" s="32"/>
-      <c r="AA1" s="32"/>
-      <c r="AB1" s="32"/>
-      <c r="AC1" s="32"/>
-      <c r="AD1" s="32"/>
-      <c r="AE1" s="32"/>
-      <c r="AF1" s="32"/>
-      <c r="AG1" s="32"/>
-      <c r="AH1" s="32"/>
-      <c r="AI1" s="32"/>
-      <c r="AJ1" s="32"/>
-      <c r="AK1" s="32"/>
-      <c r="AL1" s="32"/>
-      <c r="AM1" s="32"/>
-      <c r="AN1" s="32"/>
-      <c r="AO1" s="32"/>
-      <c r="AP1" s="32"/>
-      <c r="AQ1" s="32"/>
-      <c r="AR1" s="32"/>
-      <c r="AS1" s="32"/>
-      <c r="AT1" s="32"/>
-      <c r="AU1" s="32"/>
-      <c r="AV1" s="32"/>
-      <c r="AW1" s="32"/>
-      <c r="AX1" s="32"/>
-      <c r="AY1" s="32"/>
-      <c r="AZ1" s="32"/>
-      <c r="BA1" s="32"/>
-      <c r="BB1" s="32"/>
-      <c r="BC1" s="32"/>
-      <c r="BD1" s="32"/>
-      <c r="BE1" s="32"/>
-      <c r="BF1" s="32"/>
-      <c r="BG1" s="32"/>
-      <c r="BH1" s="32"/>
-      <c r="BI1" s="32"/>
-      <c r="BJ1" s="32"/>
-      <c r="BK1" s="32"/>
-      <c r="BL1" s="32"/>
-      <c r="BM1" s="32"/>
-      <c r="BN1" s="32"/>
-      <c r="BO1" s="32"/>
-      <c r="BP1" s="32"/>
-      <c r="BQ1" s="32"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
+      <c r="P1" s="35"/>
+      <c r="Q1" s="35"/>
+      <c r="R1" s="35"/>
+      <c r="S1" s="35"/>
+      <c r="T1" s="35"/>
+      <c r="U1" s="35"/>
+      <c r="V1" s="35"/>
+      <c r="W1" s="35"/>
+      <c r="X1" s="35"/>
+      <c r="Y1" s="35"/>
+      <c r="Z1" s="35"/>
+      <c r="AA1" s="35"/>
+      <c r="AB1" s="35"/>
+      <c r="AC1" s="35"/>
+      <c r="AD1" s="35"/>
+      <c r="AE1" s="35"/>
+      <c r="AF1" s="35"/>
+      <c r="AG1" s="35"/>
+      <c r="AH1" s="35"/>
+      <c r="AI1" s="35"/>
+      <c r="AJ1" s="35"/>
+      <c r="AK1" s="35"/>
+      <c r="AL1" s="35"/>
+      <c r="AM1" s="35"/>
+      <c r="AN1" s="35"/>
+      <c r="AO1" s="35"/>
+      <c r="AP1" s="35"/>
+      <c r="AQ1" s="35"/>
+      <c r="AR1" s="35"/>
+      <c r="AS1" s="35"/>
+      <c r="AT1" s="35"/>
+      <c r="AU1" s="35"/>
+      <c r="AV1" s="35"/>
+      <c r="AW1" s="35"/>
+      <c r="AX1" s="35"/>
+      <c r="AY1" s="35"/>
+      <c r="AZ1" s="35"/>
+      <c r="BA1" s="35"/>
+      <c r="BB1" s="35"/>
+      <c r="BC1" s="35"/>
+      <c r="BD1" s="35"/>
+      <c r="BE1" s="35"/>
+      <c r="BF1" s="35"/>
+      <c r="BG1" s="35"/>
+      <c r="BH1" s="35"/>
+      <c r="BI1" s="35"/>
+      <c r="BJ1" s="35"/>
+      <c r="BK1" s="35"/>
+      <c r="BL1" s="35"/>
+      <c r="BM1" s="35"/>
+      <c r="BN1" s="35"/>
+      <c r="BO1" s="35"/>
+      <c r="BP1" s="35"/>
+      <c r="BQ1" s="35"/>
     </row>
     <row r="2" spans="1:69">
       <c r="A2" s="10" t="s">
@@ -4374,11 +4452,11 @@
       </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="32"/>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
+      <c r="A28" s="35"/>
+      <c r="B28" s="35"/>
+      <c r="C28" s="35"/>
+      <c r="D28" s="35"/>
+      <c r="E28" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -4398,8 +4476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D234"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView topLeftCell="A18" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -4710,7 +4788,9 @@
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="B34" s="6"/>
+      <c r="B34" s="6" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="5">
@@ -5750,72 +5830,72 @@
       <c r="E1" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="32"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="32"/>
-      <c r="X1" s="32"/>
-      <c r="Y1" s="32"/>
-      <c r="Z1" s="32"/>
-      <c r="AA1" s="32"/>
-      <c r="AB1" s="32"/>
-      <c r="AC1" s="32"/>
-      <c r="AD1" s="32"/>
-      <c r="AE1" s="32"/>
-      <c r="AF1" s="32"/>
-      <c r="AG1" s="32"/>
-      <c r="AH1" s="32"/>
-      <c r="AI1" s="32"/>
-      <c r="AJ1" s="32"/>
-      <c r="AK1" s="32"/>
-      <c r="AL1" s="32"/>
-      <c r="AM1" s="32"/>
-      <c r="AN1" s="32"/>
-      <c r="AO1" s="32"/>
-      <c r="AP1" s="32"/>
-      <c r="AQ1" s="32"/>
-      <c r="AR1" s="32"/>
-      <c r="AS1" s="32"/>
-      <c r="AT1" s="32"/>
-      <c r="AU1" s="32"/>
-      <c r="AV1" s="32"/>
-      <c r="AW1" s="32"/>
-      <c r="AX1" s="32"/>
-      <c r="AY1" s="32"/>
-      <c r="AZ1" s="32"/>
-      <c r="BA1" s="32"/>
-      <c r="BB1" s="32"/>
-      <c r="BC1" s="32"/>
-      <c r="BD1" s="32"/>
-      <c r="BE1" s="32"/>
-      <c r="BF1" s="32"/>
-      <c r="BG1" s="32"/>
-      <c r="BH1" s="32"/>
-      <c r="BI1" s="32"/>
-      <c r="BJ1" s="32"/>
-      <c r="BK1" s="32"/>
-      <c r="BL1" s="32"/>
-      <c r="BM1" s="32"/>
-      <c r="BN1" s="32"/>
-      <c r="BO1" s="32"/>
-      <c r="BP1" s="32"/>
-      <c r="BQ1" s="32"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
+      <c r="P1" s="35"/>
+      <c r="Q1" s="35"/>
+      <c r="R1" s="35"/>
+      <c r="S1" s="35"/>
+      <c r="T1" s="35"/>
+      <c r="U1" s="35"/>
+      <c r="V1" s="35"/>
+      <c r="W1" s="35"/>
+      <c r="X1" s="35"/>
+      <c r="Y1" s="35"/>
+      <c r="Z1" s="35"/>
+      <c r="AA1" s="35"/>
+      <c r="AB1" s="35"/>
+      <c r="AC1" s="35"/>
+      <c r="AD1" s="35"/>
+      <c r="AE1" s="35"/>
+      <c r="AF1" s="35"/>
+      <c r="AG1" s="35"/>
+      <c r="AH1" s="35"/>
+      <c r="AI1" s="35"/>
+      <c r="AJ1" s="35"/>
+      <c r="AK1" s="35"/>
+      <c r="AL1" s="35"/>
+      <c r="AM1" s="35"/>
+      <c r="AN1" s="35"/>
+      <c r="AO1" s="35"/>
+      <c r="AP1" s="35"/>
+      <c r="AQ1" s="35"/>
+      <c r="AR1" s="35"/>
+      <c r="AS1" s="35"/>
+      <c r="AT1" s="35"/>
+      <c r="AU1" s="35"/>
+      <c r="AV1" s="35"/>
+      <c r="AW1" s="35"/>
+      <c r="AX1" s="35"/>
+      <c r="AY1" s="35"/>
+      <c r="AZ1" s="35"/>
+      <c r="BA1" s="35"/>
+      <c r="BB1" s="35"/>
+      <c r="BC1" s="35"/>
+      <c r="BD1" s="35"/>
+      <c r="BE1" s="35"/>
+      <c r="BF1" s="35"/>
+      <c r="BG1" s="35"/>
+      <c r="BH1" s="35"/>
+      <c r="BI1" s="35"/>
+      <c r="BJ1" s="35"/>
+      <c r="BK1" s="35"/>
+      <c r="BL1" s="35"/>
+      <c r="BM1" s="35"/>
+      <c r="BN1" s="35"/>
+      <c r="BO1" s="35"/>
+      <c r="BP1" s="35"/>
+      <c r="BQ1" s="35"/>
     </row>
     <row r="2" spans="1:69">
       <c r="A2" s="4" t="s">
@@ -6131,13 +6211,13 @@
       </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="32" t="s">
+      <c r="A29" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="B29" s="32"/>
-      <c r="C29" s="32"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="32"/>
+      <c r="B29" s="35"/>
+      <c r="C29" s="35"/>
+      <c r="D29" s="35"/>
+      <c r="E29" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -6186,72 +6266,72 @@
       <c r="D1" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="32"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="32"/>
-      <c r="X1" s="32"/>
-      <c r="Y1" s="32"/>
-      <c r="Z1" s="32"/>
-      <c r="AA1" s="32"/>
-      <c r="AB1" s="32"/>
-      <c r="AC1" s="32"/>
-      <c r="AD1" s="32"/>
-      <c r="AE1" s="32"/>
-      <c r="AF1" s="32"/>
-      <c r="AG1" s="32"/>
-      <c r="AH1" s="32"/>
-      <c r="AI1" s="32"/>
-      <c r="AJ1" s="32"/>
-      <c r="AK1" s="32"/>
-      <c r="AL1" s="32"/>
-      <c r="AM1" s="32"/>
-      <c r="AN1" s="32"/>
-      <c r="AO1" s="32"/>
-      <c r="AP1" s="32"/>
-      <c r="AQ1" s="32"/>
-      <c r="AR1" s="32"/>
-      <c r="AS1" s="32"/>
-      <c r="AT1" s="32"/>
-      <c r="AU1" s="32"/>
-      <c r="AV1" s="32"/>
-      <c r="AW1" s="32"/>
-      <c r="AX1" s="32"/>
-      <c r="AY1" s="32"/>
-      <c r="AZ1" s="32"/>
-      <c r="BA1" s="32"/>
-      <c r="BB1" s="32"/>
-      <c r="BC1" s="32"/>
-      <c r="BD1" s="32"/>
-      <c r="BE1" s="32"/>
-      <c r="BF1" s="32"/>
-      <c r="BG1" s="32"/>
-      <c r="BH1" s="32"/>
-      <c r="BI1" s="32"/>
-      <c r="BJ1" s="32"/>
-      <c r="BK1" s="32"/>
-      <c r="BL1" s="32"/>
-      <c r="BM1" s="32"/>
-      <c r="BN1" s="32"/>
-      <c r="BO1" s="32"/>
-      <c r="BP1" s="32"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
+      <c r="P1" s="35"/>
+      <c r="Q1" s="35"/>
+      <c r="R1" s="35"/>
+      <c r="S1" s="35"/>
+      <c r="T1" s="35"/>
+      <c r="U1" s="35"/>
+      <c r="V1" s="35"/>
+      <c r="W1" s="35"/>
+      <c r="X1" s="35"/>
+      <c r="Y1" s="35"/>
+      <c r="Z1" s="35"/>
+      <c r="AA1" s="35"/>
+      <c r="AB1" s="35"/>
+      <c r="AC1" s="35"/>
+      <c r="AD1" s="35"/>
+      <c r="AE1" s="35"/>
+      <c r="AF1" s="35"/>
+      <c r="AG1" s="35"/>
+      <c r="AH1" s="35"/>
+      <c r="AI1" s="35"/>
+      <c r="AJ1" s="35"/>
+      <c r="AK1" s="35"/>
+      <c r="AL1" s="35"/>
+      <c r="AM1" s="35"/>
+      <c r="AN1" s="35"/>
+      <c r="AO1" s="35"/>
+      <c r="AP1" s="35"/>
+      <c r="AQ1" s="35"/>
+      <c r="AR1" s="35"/>
+      <c r="AS1" s="35"/>
+      <c r="AT1" s="35"/>
+      <c r="AU1" s="35"/>
+      <c r="AV1" s="35"/>
+      <c r="AW1" s="35"/>
+      <c r="AX1" s="35"/>
+      <c r="AY1" s="35"/>
+      <c r="AZ1" s="35"/>
+      <c r="BA1" s="35"/>
+      <c r="BB1" s="35"/>
+      <c r="BC1" s="35"/>
+      <c r="BD1" s="35"/>
+      <c r="BE1" s="35"/>
+      <c r="BF1" s="35"/>
+      <c r="BG1" s="35"/>
+      <c r="BH1" s="35"/>
+      <c r="BI1" s="35"/>
+      <c r="BJ1" s="35"/>
+      <c r="BK1" s="35"/>
+      <c r="BL1" s="35"/>
+      <c r="BM1" s="35"/>
+      <c r="BN1" s="35"/>
+      <c r="BO1" s="35"/>
+      <c r="BP1" s="35"/>
     </row>
     <row r="2" spans="1:68">
       <c r="A2" s="9" t="s">
@@ -6758,7 +6838,7 @@
       <c r="C44" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="D44" s="33" t="s">
+      <c r="D44" s="30" t="s">
         <v>221</v>
       </c>
     </row>
@@ -6773,13 +6853,13 @@
       <c r="C45" s="8" t="s">
         <v>226</v>
       </c>
-      <c r="D45" s="34" t="s">
+      <c r="D45" s="31" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="3">
-        <f t="shared" ref="A46:A54" si="1">A45+1</f>
+        <f t="shared" ref="A46" si="1">A45+1</f>
         <v>2</v>
       </c>
       <c r="B46" s="3" t="s">
@@ -6788,7 +6868,7 @@
       <c r="C46" s="8">
         <v>25</v>
       </c>
-      <c r="D46" s="34" t="s">
+      <c r="D46" s="31" t="s">
         <v>155</v>
       </c>
     </row>
@@ -6800,7 +6880,6 @@
     <mergeCell ref="E1:BP1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -6841,72 +6920,72 @@
       <c r="D1" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="32"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="32"/>
-      <c r="X1" s="32"/>
-      <c r="Y1" s="32"/>
-      <c r="Z1" s="32"/>
-      <c r="AA1" s="32"/>
-      <c r="AB1" s="32"/>
-      <c r="AC1" s="32"/>
-      <c r="AD1" s="32"/>
-      <c r="AE1" s="32"/>
-      <c r="AF1" s="32"/>
-      <c r="AG1" s="32"/>
-      <c r="AH1" s="32"/>
-      <c r="AI1" s="32"/>
-      <c r="AJ1" s="32"/>
-      <c r="AK1" s="32"/>
-      <c r="AL1" s="32"/>
-      <c r="AM1" s="32"/>
-      <c r="AN1" s="32"/>
-      <c r="AO1" s="32"/>
-      <c r="AP1" s="32"/>
-      <c r="AQ1" s="32"/>
-      <c r="AR1" s="32"/>
-      <c r="AS1" s="32"/>
-      <c r="AT1" s="32"/>
-      <c r="AU1" s="32"/>
-      <c r="AV1" s="32"/>
-      <c r="AW1" s="32"/>
-      <c r="AX1" s="32"/>
-      <c r="AY1" s="32"/>
-      <c r="AZ1" s="32"/>
-      <c r="BA1" s="32"/>
-      <c r="BB1" s="32"/>
-      <c r="BC1" s="32"/>
-      <c r="BD1" s="32"/>
-      <c r="BE1" s="32"/>
-      <c r="BF1" s="32"/>
-      <c r="BG1" s="32"/>
-      <c r="BH1" s="32"/>
-      <c r="BI1" s="32"/>
-      <c r="BJ1" s="32"/>
-      <c r="BK1" s="32"/>
-      <c r="BL1" s="32"/>
-      <c r="BM1" s="32"/>
-      <c r="BN1" s="32"/>
-      <c r="BO1" s="32"/>
-      <c r="BP1" s="32"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
+      <c r="P1" s="35"/>
+      <c r="Q1" s="35"/>
+      <c r="R1" s="35"/>
+      <c r="S1" s="35"/>
+      <c r="T1" s="35"/>
+      <c r="U1" s="35"/>
+      <c r="V1" s="35"/>
+      <c r="W1" s="35"/>
+      <c r="X1" s="35"/>
+      <c r="Y1" s="35"/>
+      <c r="Z1" s="35"/>
+      <c r="AA1" s="35"/>
+      <c r="AB1" s="35"/>
+      <c r="AC1" s="35"/>
+      <c r="AD1" s="35"/>
+      <c r="AE1" s="35"/>
+      <c r="AF1" s="35"/>
+      <c r="AG1" s="35"/>
+      <c r="AH1" s="35"/>
+      <c r="AI1" s="35"/>
+      <c r="AJ1" s="35"/>
+      <c r="AK1" s="35"/>
+      <c r="AL1" s="35"/>
+      <c r="AM1" s="35"/>
+      <c r="AN1" s="35"/>
+      <c r="AO1" s="35"/>
+      <c r="AP1" s="35"/>
+      <c r="AQ1" s="35"/>
+      <c r="AR1" s="35"/>
+      <c r="AS1" s="35"/>
+      <c r="AT1" s="35"/>
+      <c r="AU1" s="35"/>
+      <c r="AV1" s="35"/>
+      <c r="AW1" s="35"/>
+      <c r="AX1" s="35"/>
+      <c r="AY1" s="35"/>
+      <c r="AZ1" s="35"/>
+      <c r="BA1" s="35"/>
+      <c r="BB1" s="35"/>
+      <c r="BC1" s="35"/>
+      <c r="BD1" s="35"/>
+      <c r="BE1" s="35"/>
+      <c r="BF1" s="35"/>
+      <c r="BG1" s="35"/>
+      <c r="BH1" s="35"/>
+      <c r="BI1" s="35"/>
+      <c r="BJ1" s="35"/>
+      <c r="BK1" s="35"/>
+      <c r="BL1" s="35"/>
+      <c r="BM1" s="35"/>
+      <c r="BN1" s="35"/>
+      <c r="BO1" s="35"/>
+      <c r="BP1" s="35"/>
     </row>
     <row r="2" spans="1:68">
       <c r="A2" s="9" t="s">
@@ -7035,10 +7114,10 @@
       </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="32"/>
-      <c r="B29" s="32"/>
-      <c r="C29" s="32"/>
-      <c r="D29" s="32"/>
+      <c r="A29" s="35"/>
+      <c r="B29" s="35"/>
+      <c r="C29" s="35"/>
+      <c r="D29" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -7086,72 +7165,72 @@
       <c r="D1" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="32"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="32"/>
-      <c r="X1" s="32"/>
-      <c r="Y1" s="32"/>
-      <c r="Z1" s="32"/>
-      <c r="AA1" s="32"/>
-      <c r="AB1" s="32"/>
-      <c r="AC1" s="32"/>
-      <c r="AD1" s="32"/>
-      <c r="AE1" s="32"/>
-      <c r="AF1" s="32"/>
-      <c r="AG1" s="32"/>
-      <c r="AH1" s="32"/>
-      <c r="AI1" s="32"/>
-      <c r="AJ1" s="32"/>
-      <c r="AK1" s="32"/>
-      <c r="AL1" s="32"/>
-      <c r="AM1" s="32"/>
-      <c r="AN1" s="32"/>
-      <c r="AO1" s="32"/>
-      <c r="AP1" s="32"/>
-      <c r="AQ1" s="32"/>
-      <c r="AR1" s="32"/>
-      <c r="AS1" s="32"/>
-      <c r="AT1" s="32"/>
-      <c r="AU1" s="32"/>
-      <c r="AV1" s="32"/>
-      <c r="AW1" s="32"/>
-      <c r="AX1" s="32"/>
-      <c r="AY1" s="32"/>
-      <c r="AZ1" s="32"/>
-      <c r="BA1" s="32"/>
-      <c r="BB1" s="32"/>
-      <c r="BC1" s="32"/>
-      <c r="BD1" s="32"/>
-      <c r="BE1" s="32"/>
-      <c r="BF1" s="32"/>
-      <c r="BG1" s="32"/>
-      <c r="BH1" s="32"/>
-      <c r="BI1" s="32"/>
-      <c r="BJ1" s="32"/>
-      <c r="BK1" s="32"/>
-      <c r="BL1" s="32"/>
-      <c r="BM1" s="32"/>
-      <c r="BN1" s="32"/>
-      <c r="BO1" s="32"/>
-      <c r="BP1" s="32"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
+      <c r="P1" s="35"/>
+      <c r="Q1" s="35"/>
+      <c r="R1" s="35"/>
+      <c r="S1" s="35"/>
+      <c r="T1" s="35"/>
+      <c r="U1" s="35"/>
+      <c r="V1" s="35"/>
+      <c r="W1" s="35"/>
+      <c r="X1" s="35"/>
+      <c r="Y1" s="35"/>
+      <c r="Z1" s="35"/>
+      <c r="AA1" s="35"/>
+      <c r="AB1" s="35"/>
+      <c r="AC1" s="35"/>
+      <c r="AD1" s="35"/>
+      <c r="AE1" s="35"/>
+      <c r="AF1" s="35"/>
+      <c r="AG1" s="35"/>
+      <c r="AH1" s="35"/>
+      <c r="AI1" s="35"/>
+      <c r="AJ1" s="35"/>
+      <c r="AK1" s="35"/>
+      <c r="AL1" s="35"/>
+      <c r="AM1" s="35"/>
+      <c r="AN1" s="35"/>
+      <c r="AO1" s="35"/>
+      <c r="AP1" s="35"/>
+      <c r="AQ1" s="35"/>
+      <c r="AR1" s="35"/>
+      <c r="AS1" s="35"/>
+      <c r="AT1" s="35"/>
+      <c r="AU1" s="35"/>
+      <c r="AV1" s="35"/>
+      <c r="AW1" s="35"/>
+      <c r="AX1" s="35"/>
+      <c r="AY1" s="35"/>
+      <c r="AZ1" s="35"/>
+      <c r="BA1" s="35"/>
+      <c r="BB1" s="35"/>
+      <c r="BC1" s="35"/>
+      <c r="BD1" s="35"/>
+      <c r="BE1" s="35"/>
+      <c r="BF1" s="35"/>
+      <c r="BG1" s="35"/>
+      <c r="BH1" s="35"/>
+      <c r="BI1" s="35"/>
+      <c r="BJ1" s="35"/>
+      <c r="BK1" s="35"/>
+      <c r="BL1" s="35"/>
+      <c r="BM1" s="35"/>
+      <c r="BN1" s="35"/>
+      <c r="BO1" s="35"/>
+      <c r="BP1" s="35"/>
     </row>
     <row r="2" spans="1:68">
       <c r="A2" s="9" t="s">
@@ -7280,10 +7359,10 @@
       </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="32"/>
-      <c r="B29" s="32"/>
-      <c r="C29" s="32"/>
-      <c r="D29" s="32"/>
+      <c r="A29" s="35"/>
+      <c r="B29" s="35"/>
+      <c r="C29" s="35"/>
+      <c r="D29" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -7303,8 +7382,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BP28"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7331,72 +7410,72 @@
       <c r="D1" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="32"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="32"/>
-      <c r="X1" s="32"/>
-      <c r="Y1" s="32"/>
-      <c r="Z1" s="32"/>
-      <c r="AA1" s="32"/>
-      <c r="AB1" s="32"/>
-      <c r="AC1" s="32"/>
-      <c r="AD1" s="32"/>
-      <c r="AE1" s="32"/>
-      <c r="AF1" s="32"/>
-      <c r="AG1" s="32"/>
-      <c r="AH1" s="32"/>
-      <c r="AI1" s="32"/>
-      <c r="AJ1" s="32"/>
-      <c r="AK1" s="32"/>
-      <c r="AL1" s="32"/>
-      <c r="AM1" s="32"/>
-      <c r="AN1" s="32"/>
-      <c r="AO1" s="32"/>
-      <c r="AP1" s="32"/>
-      <c r="AQ1" s="32"/>
-      <c r="AR1" s="32"/>
-      <c r="AS1" s="32"/>
-      <c r="AT1" s="32"/>
-      <c r="AU1" s="32"/>
-      <c r="AV1" s="32"/>
-      <c r="AW1" s="32"/>
-      <c r="AX1" s="32"/>
-      <c r="AY1" s="32"/>
-      <c r="AZ1" s="32"/>
-      <c r="BA1" s="32"/>
-      <c r="BB1" s="32"/>
-      <c r="BC1" s="32"/>
-      <c r="BD1" s="32"/>
-      <c r="BE1" s="32"/>
-      <c r="BF1" s="32"/>
-      <c r="BG1" s="32"/>
-      <c r="BH1" s="32"/>
-      <c r="BI1" s="32"/>
-      <c r="BJ1" s="32"/>
-      <c r="BK1" s="32"/>
-      <c r="BL1" s="32"/>
-      <c r="BM1" s="32"/>
-      <c r="BN1" s="32"/>
-      <c r="BO1" s="32"/>
-      <c r="BP1" s="32"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
+      <c r="P1" s="35"/>
+      <c r="Q1" s="35"/>
+      <c r="R1" s="35"/>
+      <c r="S1" s="35"/>
+      <c r="T1" s="35"/>
+      <c r="U1" s="35"/>
+      <c r="V1" s="35"/>
+      <c r="W1" s="35"/>
+      <c r="X1" s="35"/>
+      <c r="Y1" s="35"/>
+      <c r="Z1" s="35"/>
+      <c r="AA1" s="35"/>
+      <c r="AB1" s="35"/>
+      <c r="AC1" s="35"/>
+      <c r="AD1" s="35"/>
+      <c r="AE1" s="35"/>
+      <c r="AF1" s="35"/>
+      <c r="AG1" s="35"/>
+      <c r="AH1" s="35"/>
+      <c r="AI1" s="35"/>
+      <c r="AJ1" s="35"/>
+      <c r="AK1" s="35"/>
+      <c r="AL1" s="35"/>
+      <c r="AM1" s="35"/>
+      <c r="AN1" s="35"/>
+      <c r="AO1" s="35"/>
+      <c r="AP1" s="35"/>
+      <c r="AQ1" s="35"/>
+      <c r="AR1" s="35"/>
+      <c r="AS1" s="35"/>
+      <c r="AT1" s="35"/>
+      <c r="AU1" s="35"/>
+      <c r="AV1" s="35"/>
+      <c r="AW1" s="35"/>
+      <c r="AX1" s="35"/>
+      <c r="AY1" s="35"/>
+      <c r="AZ1" s="35"/>
+      <c r="BA1" s="35"/>
+      <c r="BB1" s="35"/>
+      <c r="BC1" s="35"/>
+      <c r="BD1" s="35"/>
+      <c r="BE1" s="35"/>
+      <c r="BF1" s="35"/>
+      <c r="BG1" s="35"/>
+      <c r="BH1" s="35"/>
+      <c r="BI1" s="35"/>
+      <c r="BJ1" s="35"/>
+      <c r="BK1" s="35"/>
+      <c r="BL1" s="35"/>
+      <c r="BM1" s="35"/>
+      <c r="BN1" s="35"/>
+      <c r="BO1" s="35"/>
+      <c r="BP1" s="35"/>
     </row>
     <row r="2" spans="1:68">
       <c r="A2" s="10" t="s">
@@ -7483,12 +7562,24 @@
         <v>5</v>
       </c>
       <c r="B8" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="C8" s="13">
+        <v>32</v>
+      </c>
+      <c r="D8" s="11"/>
+    </row>
+    <row r="9" spans="1:68">
+      <c r="A9" s="11">
+        <v>6</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C9" s="13">
         <v>26</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D9" s="11" t="s">
         <v>155</v>
       </c>
     </row>
@@ -7498,10 +7589,10 @@
       </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="32"/>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
+      <c r="A28" s="35"/>
+      <c r="B28" s="35"/>
+      <c r="C28" s="35"/>
+      <c r="D28" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -7509,6 +7600,7 @@
     <mergeCell ref="A28:D28"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -7545,72 +7637,72 @@
       <c r="D1" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="32"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="32"/>
-      <c r="X1" s="32"/>
-      <c r="Y1" s="32"/>
-      <c r="Z1" s="32"/>
-      <c r="AA1" s="32"/>
-      <c r="AB1" s="32"/>
-      <c r="AC1" s="32"/>
-      <c r="AD1" s="32"/>
-      <c r="AE1" s="32"/>
-      <c r="AF1" s="32"/>
-      <c r="AG1" s="32"/>
-      <c r="AH1" s="32"/>
-      <c r="AI1" s="32"/>
-      <c r="AJ1" s="32"/>
-      <c r="AK1" s="32"/>
-      <c r="AL1" s="32"/>
-      <c r="AM1" s="32"/>
-      <c r="AN1" s="32"/>
-      <c r="AO1" s="32"/>
-      <c r="AP1" s="32"/>
-      <c r="AQ1" s="32"/>
-      <c r="AR1" s="32"/>
-      <c r="AS1" s="32"/>
-      <c r="AT1" s="32"/>
-      <c r="AU1" s="32"/>
-      <c r="AV1" s="32"/>
-      <c r="AW1" s="32"/>
-      <c r="AX1" s="32"/>
-      <c r="AY1" s="32"/>
-      <c r="AZ1" s="32"/>
-      <c r="BA1" s="32"/>
-      <c r="BB1" s="32"/>
-      <c r="BC1" s="32"/>
-      <c r="BD1" s="32"/>
-      <c r="BE1" s="32"/>
-      <c r="BF1" s="32"/>
-      <c r="BG1" s="32"/>
-      <c r="BH1" s="32"/>
-      <c r="BI1" s="32"/>
-      <c r="BJ1" s="32"/>
-      <c r="BK1" s="32"/>
-      <c r="BL1" s="32"/>
-      <c r="BM1" s="32"/>
-      <c r="BN1" s="32"/>
-      <c r="BO1" s="32"/>
-      <c r="BP1" s="32"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
+      <c r="P1" s="35"/>
+      <c r="Q1" s="35"/>
+      <c r="R1" s="35"/>
+      <c r="S1" s="35"/>
+      <c r="T1" s="35"/>
+      <c r="U1" s="35"/>
+      <c r="V1" s="35"/>
+      <c r="W1" s="35"/>
+      <c r="X1" s="35"/>
+      <c r="Y1" s="35"/>
+      <c r="Z1" s="35"/>
+      <c r="AA1" s="35"/>
+      <c r="AB1" s="35"/>
+      <c r="AC1" s="35"/>
+      <c r="AD1" s="35"/>
+      <c r="AE1" s="35"/>
+      <c r="AF1" s="35"/>
+      <c r="AG1" s="35"/>
+      <c r="AH1" s="35"/>
+      <c r="AI1" s="35"/>
+      <c r="AJ1" s="35"/>
+      <c r="AK1" s="35"/>
+      <c r="AL1" s="35"/>
+      <c r="AM1" s="35"/>
+      <c r="AN1" s="35"/>
+      <c r="AO1" s="35"/>
+      <c r="AP1" s="35"/>
+      <c r="AQ1" s="35"/>
+      <c r="AR1" s="35"/>
+      <c r="AS1" s="35"/>
+      <c r="AT1" s="35"/>
+      <c r="AU1" s="35"/>
+      <c r="AV1" s="35"/>
+      <c r="AW1" s="35"/>
+      <c r="AX1" s="35"/>
+      <c r="AY1" s="35"/>
+      <c r="AZ1" s="35"/>
+      <c r="BA1" s="35"/>
+      <c r="BB1" s="35"/>
+      <c r="BC1" s="35"/>
+      <c r="BD1" s="35"/>
+      <c r="BE1" s="35"/>
+      <c r="BF1" s="35"/>
+      <c r="BG1" s="35"/>
+      <c r="BH1" s="35"/>
+      <c r="BI1" s="35"/>
+      <c r="BJ1" s="35"/>
+      <c r="BK1" s="35"/>
+      <c r="BL1" s="35"/>
+      <c r="BM1" s="35"/>
+      <c r="BN1" s="35"/>
+      <c r="BO1" s="35"/>
+      <c r="BP1" s="35"/>
     </row>
     <row r="2" spans="1:68" ht="15">
       <c r="A2" s="10" t="s">
@@ -8197,72 +8289,72 @@
       <c r="D1" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="32"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="32"/>
-      <c r="X1" s="32"/>
-      <c r="Y1" s="32"/>
-      <c r="Z1" s="32"/>
-      <c r="AA1" s="32"/>
-      <c r="AB1" s="32"/>
-      <c r="AC1" s="32"/>
-      <c r="AD1" s="32"/>
-      <c r="AE1" s="32"/>
-      <c r="AF1" s="32"/>
-      <c r="AG1" s="32"/>
-      <c r="AH1" s="32"/>
-      <c r="AI1" s="32"/>
-      <c r="AJ1" s="32"/>
-      <c r="AK1" s="32"/>
-      <c r="AL1" s="32"/>
-      <c r="AM1" s="32"/>
-      <c r="AN1" s="32"/>
-      <c r="AO1" s="32"/>
-      <c r="AP1" s="32"/>
-      <c r="AQ1" s="32"/>
-      <c r="AR1" s="32"/>
-      <c r="AS1" s="32"/>
-      <c r="AT1" s="32"/>
-      <c r="AU1" s="32"/>
-      <c r="AV1" s="32"/>
-      <c r="AW1" s="32"/>
-      <c r="AX1" s="32"/>
-      <c r="AY1" s="32"/>
-      <c r="AZ1" s="32"/>
-      <c r="BA1" s="32"/>
-      <c r="BB1" s="32"/>
-      <c r="BC1" s="32"/>
-      <c r="BD1" s="32"/>
-      <c r="BE1" s="32"/>
-      <c r="BF1" s="32"/>
-      <c r="BG1" s="32"/>
-      <c r="BH1" s="32"/>
-      <c r="BI1" s="32"/>
-      <c r="BJ1" s="32"/>
-      <c r="BK1" s="32"/>
-      <c r="BL1" s="32"/>
-      <c r="BM1" s="32"/>
-      <c r="BN1" s="32"/>
-      <c r="BO1" s="32"/>
-      <c r="BP1" s="32"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
+      <c r="P1" s="35"/>
+      <c r="Q1" s="35"/>
+      <c r="R1" s="35"/>
+      <c r="S1" s="35"/>
+      <c r="T1" s="35"/>
+      <c r="U1" s="35"/>
+      <c r="V1" s="35"/>
+      <c r="W1" s="35"/>
+      <c r="X1" s="35"/>
+      <c r="Y1" s="35"/>
+      <c r="Z1" s="35"/>
+      <c r="AA1" s="35"/>
+      <c r="AB1" s="35"/>
+      <c r="AC1" s="35"/>
+      <c r="AD1" s="35"/>
+      <c r="AE1" s="35"/>
+      <c r="AF1" s="35"/>
+      <c r="AG1" s="35"/>
+      <c r="AH1" s="35"/>
+      <c r="AI1" s="35"/>
+      <c r="AJ1" s="35"/>
+      <c r="AK1" s="35"/>
+      <c r="AL1" s="35"/>
+      <c r="AM1" s="35"/>
+      <c r="AN1" s="35"/>
+      <c r="AO1" s="35"/>
+      <c r="AP1" s="35"/>
+      <c r="AQ1" s="35"/>
+      <c r="AR1" s="35"/>
+      <c r="AS1" s="35"/>
+      <c r="AT1" s="35"/>
+      <c r="AU1" s="35"/>
+      <c r="AV1" s="35"/>
+      <c r="AW1" s="35"/>
+      <c r="AX1" s="35"/>
+      <c r="AY1" s="35"/>
+      <c r="AZ1" s="35"/>
+      <c r="BA1" s="35"/>
+      <c r="BB1" s="35"/>
+      <c r="BC1" s="35"/>
+      <c r="BD1" s="35"/>
+      <c r="BE1" s="35"/>
+      <c r="BF1" s="35"/>
+      <c r="BG1" s="35"/>
+      <c r="BH1" s="35"/>
+      <c r="BI1" s="35"/>
+      <c r="BJ1" s="35"/>
+      <c r="BK1" s="35"/>
+      <c r="BL1" s="35"/>
+      <c r="BM1" s="35"/>
+      <c r="BN1" s="35"/>
+      <c r="BO1" s="35"/>
+      <c r="BP1" s="35"/>
     </row>
     <row r="2" spans="1:68">
       <c r="A2" s="10" t="s">

</xml_diff>

<commit_message>
fix jms and add nop + hlt commands
</commit_message>
<xml_diff>
--- a/doc/controls.xlsx
+++ b/doc/controls.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="20480" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="20480"/>
   </bookViews>
   <sheets>
     <sheet name="COMMANDS" sheetId="3" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="235">
   <si>
     <t>#</t>
   </si>
@@ -2688,8 +2688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3353,7 +3353,7 @@
         <v>0</v>
       </c>
       <c r="K13" s="17" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="L13" s="16" t="str">
         <f t="shared" si="2"/>
@@ -3365,7 +3365,7 @@
       </c>
       <c r="N13" s="11" t="str">
         <f t="shared" si="8"/>
-        <v>0004</v>
+        <v>0008</v>
       </c>
       <c r="O13" s="11" t="str">
         <f t="shared" si="5"/>
@@ -3449,7 +3449,7 @@
         <v>0</v>
       </c>
       <c r="K15" s="17" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="L15" s="16" t="str">
         <f t="shared" si="2"/>
@@ -3461,7 +3461,7 @@
       </c>
       <c r="N15" s="11" t="str">
         <f t="shared" si="8"/>
-        <v>0008</v>
+        <v>0004</v>
       </c>
       <c r="O15" s="11" t="str">
         <f t="shared" si="5"/>
@@ -4476,8 +4476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D234"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView topLeftCell="A22" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -4797,7 +4797,9 @@
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="B35" s="6"/>
+      <c r="B35" s="6" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="5">
@@ -7382,7 +7384,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BP28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>

</xml_diff>